<commit_message>
Enable agency users to request more slots for shopping and places
Adds a SlotQuotaRequest model and UI templates for agencies to request slot quotas.

Replit-Commit-Author: Agent
Replit-Commit-Session-Id: 1ee98367-f536-4fd9-b794-de0a132696f6
Replit-Commit-Screenshot-Url: https://storage.googleapis.com/screenshot-production-us-central1/05c521f5-5ca3-43ca-9dcf-01c0c163b8b7/a63841d7-b72a-486a-b232-ad1f9a8122f4.jpg
</commit_message>
<xml_diff>
--- a/uploads/shopping_slots_export.xlsx
+++ b/uploads/shopping_slots_export.xlsx
@@ -16,10 +16,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="yyyy-mm-dd h:mm:ss"/>
-    <numFmt numFmtId="165" formatCode="YYYY-MM-DD HH:MM:SS"/>
-  </numFmts>
+  <numFmts count="0"/>
   <fonts count="2">
     <font>
       <name val="Calibri"/>
@@ -58,12 +55,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -429,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K3"/>
+  <dimension ref="A1:M1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -445,147 +441,63 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>대행사</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
           <t>스토어 타입</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>상품 ID</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>상품명</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>키워드</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>가격</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>할인가</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>시작일</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>종료일</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>입찰방식</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>상태</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>슬롯 단가</t>
         </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>샘플 슬롯 1</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>스마트스토어</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>P12345</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>샘플 상품 1</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>키워드1,키워드2</t>
-        </is>
-      </c>
-      <c r="F2" t="n">
-        <v>10000</v>
-      </c>
-      <c r="G2" t="n">
-        <v>8000</v>
-      </c>
-      <c r="H2" s="2" t="n">
-        <v>45778</v>
-      </c>
-      <c r="I2" s="2" t="n">
-        <v>45808</v>
-      </c>
-      <c r="J2" t="inlineStr">
-        <is>
-          <t>CPC</t>
-        </is>
-      </c>
-      <c r="K2" t="n">
-        <v>5000</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>샘플 슬롯 2</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>브랜드몰</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>P67890</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>샘플 상품 2</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>키워드3,키워드4</t>
-        </is>
-      </c>
-      <c r="F3" t="n">
-        <v>20000</v>
-      </c>
-      <c r="G3" t="n">
-        <v>18000</v>
-      </c>
-      <c r="H3" s="2" t="n">
-        <v>45792</v>
-      </c>
-      <c r="I3" s="2" t="n">
-        <v>45823</v>
-      </c>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t>CPM</t>
-        </is>
-      </c>
-      <c r="K3" t="n">
-        <v>6000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Enable agencies to manage and select shopping slots with quotas
Implement shopping slot management features with quota limits, selection, and editing in `app.py` and `templates/agency/shopping_slots.html`.

Replit-Commit-Author: Agent
Replit-Commit-Session-Id: 1ee98367-f536-4fd9-b794-de0a132696f6
Replit-Commit-Screenshot-Url: https://storage.googleapis.com/screenshot-production-us-central1/05c521f5-5ca3-43ca-9dcf-01c0c163b8b7/dc4cec88-197f-4fc3-bb21-fd0348d3045c.jpg
</commit_message>
<xml_diff>
--- a/uploads/shopping_slots_export.xlsx
+++ b/uploads/shopping_slots_export.xlsx
@@ -16,7 +16,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="yyyy-mm-dd h:mm:ss"/>
+    <numFmt numFmtId="165" formatCode="YYYY-MM-DD HH:MM:SS"/>
+  </numFmts>
   <fonts count="2">
     <font>
       <name val="Calibri"/>
@@ -55,11 +58,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -425,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M1"/>
+  <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -441,63 +445,147 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>대행사</t>
+          <t>스토어 타입</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>스토어 타입</t>
+          <t>상품 ID</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>상품 ID</t>
+          <t>상품명</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>상품명</t>
+          <t>키워드</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>키워드</t>
+          <t>가격</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>가격</t>
+          <t>할인가</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>할인가</t>
+          <t>시작일</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>시작일</t>
+          <t>종료일</t>
         </is>
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
-          <t>종료일</t>
+          <t>입찰방식</t>
         </is>
       </c>
       <c r="K1" s="1" t="inlineStr">
         <is>
-          <t>입찰방식</t>
-        </is>
-      </c>
-      <c r="L1" s="1" t="inlineStr">
-        <is>
-          <t>상태</t>
-        </is>
-      </c>
-      <c r="M1" s="1" t="inlineStr">
-        <is>
           <t>슬롯 단가</t>
         </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>샘플 슬롯 1</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>스마트스토어</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>P12345</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>샘플 상품 1</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>키워드1,키워드2</t>
+        </is>
+      </c>
+      <c r="F2" t="n">
+        <v>10000</v>
+      </c>
+      <c r="G2" t="n">
+        <v>8000</v>
+      </c>
+      <c r="H2" s="2" t="n">
+        <v>45778</v>
+      </c>
+      <c r="I2" s="2" t="n">
+        <v>45808</v>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>CPC</t>
+        </is>
+      </c>
+      <c r="K2" t="n">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>샘플 슬롯 2</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>브랜드몰</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>P67890</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>샘플 상품 2</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>키워드3,키워드4</t>
+        </is>
+      </c>
+      <c r="F3" t="n">
+        <v>20000</v>
+      </c>
+      <c r="G3" t="n">
+        <v>18000</v>
+      </c>
+      <c r="H3" s="2" t="n">
+        <v>45792</v>
+      </c>
+      <c r="I3" s="2" t="n">
+        <v>45823</v>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>CPM</t>
+        </is>
+      </c>
+      <c r="K3" t="n">
+        <v>6000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Enable distributors to manage slot activation and improve slot display
Adds slot activation toggle, reorders and renames slot list fields, and adds supporting images.

Replit-Commit-Author: Agent
Replit-Commit-Session-Id: 1ee98367-f536-4fd9-b794-de0a132696f6
Replit-Commit-Screenshot-Url: https://storage.googleapis.com/screenshot-production-us-central1/05c521f5-5ca3-43ca-9dcf-01c0c163b8b7/ef5a01ff-86a4-44b8-8778-ebe5e6b97aba.jpg
</commit_message>
<xml_diff>
--- a/uploads/shopping_slots_export.xlsx
+++ b/uploads/shopping_slots_export.xlsx
@@ -17,8 +17,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="yyyy-mm-dd h:mm:ss"/>
-    <numFmt numFmtId="165" formatCode="YYYY-MM-DD HH:MM:SS"/>
+    <numFmt numFmtId="164" formatCode="yyyy-mm-dd"/>
+    <numFmt numFmtId="165" formatCode="YYYY-MM-DD"/>
   </numFmts>
   <fonts count="2">
     <font>
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K3"/>
+  <dimension ref="A1:M11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -445,50 +445,60 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>대행사</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
           <t>스토어 타입</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>상품 ID</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>상품명</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>키워드</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>가격</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>할인가</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>시작일</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>종료일</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>입찰방식</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>상태</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>슬롯 단가</t>
         </is>
@@ -497,95 +507,331 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>샘플 슬롯 1</t>
+          <t>이이이 Shopping 슬롯 20250506-1</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>스마트스토어</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>P12345</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>샘플 상품 1</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>키워드1,키워드2</t>
-        </is>
-      </c>
-      <c r="F2" t="n">
-        <v>10000</v>
-      </c>
-      <c r="G2" t="n">
-        <v>8000</v>
-      </c>
-      <c r="H2" s="2" t="n">
-        <v>45778</v>
-      </c>
+          <t>이이이</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr"/>
+      <c r="D2" t="inlineStr"/>
+      <c r="E2" t="inlineStr"/>
+      <c r="F2" t="inlineStr"/>
+      <c r="G2" t="inlineStr"/>
+      <c r="H2" t="inlineStr"/>
       <c r="I2" s="2" t="n">
-        <v>45808</v>
-      </c>
-      <c r="J2" t="inlineStr">
-        <is>
-          <t>CPC</t>
-        </is>
-      </c>
-      <c r="K2" t="n">
-        <v>5000</v>
+        <v>45784</v>
+      </c>
+      <c r="J2" s="2" t="n">
+        <v>45786</v>
+      </c>
+      <c r="K2" t="inlineStr"/>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>live</t>
+        </is>
+      </c>
+      <c r="M2" t="n">
+        <v>30</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>샘플 슬롯 2</t>
+          <t>이이이 Shopping 슬롯 20250506-2</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>브랜드몰</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>P67890</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>샘플 상품 2</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>키워드3,키워드4</t>
-        </is>
-      </c>
-      <c r="F3" t="n">
-        <v>20000</v>
-      </c>
-      <c r="G3" t="n">
-        <v>18000</v>
-      </c>
-      <c r="H3" s="2" t="n">
-        <v>45792</v>
-      </c>
+          <t>이이이</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr"/>
+      <c r="D3" t="inlineStr"/>
+      <c r="E3" t="inlineStr"/>
+      <c r="F3" t="inlineStr"/>
+      <c r="G3" t="inlineStr"/>
+      <c r="H3" t="inlineStr"/>
       <c r="I3" s="2" t="n">
-        <v>45823</v>
-      </c>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t>CPM</t>
-        </is>
-      </c>
-      <c r="K3" t="n">
-        <v>6000</v>
+        <v>45784</v>
+      </c>
+      <c r="J3" s="2" t="n">
+        <v>45786</v>
+      </c>
+      <c r="K3" t="inlineStr"/>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>live</t>
+        </is>
+      </c>
+      <c r="M3" t="n">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>이이이 Shopping 슬롯 20250506-3</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>이이이</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr"/>
+      <c r="D4" t="inlineStr"/>
+      <c r="E4" t="inlineStr"/>
+      <c r="F4" t="inlineStr"/>
+      <c r="G4" t="inlineStr"/>
+      <c r="H4" t="inlineStr"/>
+      <c r="I4" s="2" t="n">
+        <v>45784</v>
+      </c>
+      <c r="J4" s="2" t="n">
+        <v>45786</v>
+      </c>
+      <c r="K4" t="inlineStr"/>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>live</t>
+        </is>
+      </c>
+      <c r="M4" t="n">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>이이이 Shopping 슬롯 20250506-4</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>이이이</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr"/>
+      <c r="D5" t="inlineStr"/>
+      <c r="E5" t="inlineStr"/>
+      <c r="F5" t="inlineStr"/>
+      <c r="G5" t="inlineStr"/>
+      <c r="H5" t="inlineStr"/>
+      <c r="I5" s="2" t="n">
+        <v>45784</v>
+      </c>
+      <c r="J5" s="2" t="n">
+        <v>45786</v>
+      </c>
+      <c r="K5" t="inlineStr"/>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>live</t>
+        </is>
+      </c>
+      <c r="M5" t="n">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>이이이 Shopping 슬롯 20250506-5</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>이이이</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr"/>
+      <c r="D6" t="inlineStr"/>
+      <c r="E6" t="inlineStr"/>
+      <c r="F6" t="inlineStr"/>
+      <c r="G6" t="inlineStr"/>
+      <c r="H6" t="inlineStr"/>
+      <c r="I6" s="2" t="n">
+        <v>45784</v>
+      </c>
+      <c r="J6" s="2" t="n">
+        <v>45786</v>
+      </c>
+      <c r="K6" t="inlineStr"/>
+      <c r="L6" t="inlineStr">
+        <is>
+          <t>live</t>
+        </is>
+      </c>
+      <c r="M6" t="n">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>이이이 Shopping 슬롯 20250506-6</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>이이이</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr"/>
+      <c r="D7" t="inlineStr"/>
+      <c r="E7" t="inlineStr"/>
+      <c r="F7" t="inlineStr"/>
+      <c r="G7" t="inlineStr"/>
+      <c r="H7" t="inlineStr"/>
+      <c r="I7" s="2" t="n">
+        <v>45784</v>
+      </c>
+      <c r="J7" s="2" t="n">
+        <v>45786</v>
+      </c>
+      <c r="K7" t="inlineStr"/>
+      <c r="L7" t="inlineStr">
+        <is>
+          <t>live</t>
+        </is>
+      </c>
+      <c r="M7" t="n">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>이이이 Shopping 슬롯 20250506-7</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>이이이</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr"/>
+      <c r="D8" t="inlineStr"/>
+      <c r="E8" t="inlineStr"/>
+      <c r="F8" t="inlineStr"/>
+      <c r="G8" t="inlineStr"/>
+      <c r="H8" t="inlineStr"/>
+      <c r="I8" s="2" t="n">
+        <v>45784</v>
+      </c>
+      <c r="J8" s="2" t="n">
+        <v>45786</v>
+      </c>
+      <c r="K8" t="inlineStr"/>
+      <c r="L8" t="inlineStr">
+        <is>
+          <t>live</t>
+        </is>
+      </c>
+      <c r="M8" t="n">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>이이이 Shopping 슬롯 20250506-8</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>이이이</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr"/>
+      <c r="D9" t="inlineStr"/>
+      <c r="E9" t="inlineStr"/>
+      <c r="F9" t="inlineStr"/>
+      <c r="G9" t="inlineStr"/>
+      <c r="H9" t="inlineStr"/>
+      <c r="I9" s="2" t="n">
+        <v>45784</v>
+      </c>
+      <c r="J9" s="2" t="n">
+        <v>45786</v>
+      </c>
+      <c r="K9" t="inlineStr"/>
+      <c r="L9" t="inlineStr">
+        <is>
+          <t>live</t>
+        </is>
+      </c>
+      <c r="M9" t="n">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>이이이 Shopping 슬롯 20250506-9</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>이이이</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr"/>
+      <c r="D10" t="inlineStr"/>
+      <c r="E10" t="inlineStr"/>
+      <c r="F10" t="inlineStr"/>
+      <c r="G10" t="inlineStr"/>
+      <c r="H10" t="inlineStr"/>
+      <c r="I10" s="2" t="n">
+        <v>45784</v>
+      </c>
+      <c r="J10" s="2" t="n">
+        <v>45786</v>
+      </c>
+      <c r="K10" t="inlineStr"/>
+      <c r="L10" t="inlineStr">
+        <is>
+          <t>live</t>
+        </is>
+      </c>
+      <c r="M10" t="n">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>이이이 Shopping 슬롯 20250506-10</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>이이이</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr"/>
+      <c r="D11" t="inlineStr"/>
+      <c r="E11" t="inlineStr"/>
+      <c r="F11" t="inlineStr"/>
+      <c r="G11" t="inlineStr"/>
+      <c r="H11" t="inlineStr"/>
+      <c r="I11" s="2" t="n">
+        <v>45784</v>
+      </c>
+      <c r="J11" s="2" t="n">
+        <v>45786</v>
+      </c>
+      <c r="K11" t="inlineStr"/>
+      <c r="L11" t="inlineStr">
+        <is>
+          <t>live</t>
+        </is>
+      </c>
+      <c r="M11" t="n">
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update the shopping slots spreadsheet template with new refund options
Modify uploads/shopping_slots_export.xlsx to include columns related to refunds.

Replit-Commit-Author: Agent
Replit-Commit-Session-Id: 1ee98367-f536-4fd9-b794-de0a132696f6
Replit-Commit-Screenshot-Url: https://storage.googleapis.com/screenshot-production-us-central1/05c521f5-5ca3-43ca-9dcf-01c0c163b8b7/aa685668-a263-4756-819f-87d7109a520b.jpg
</commit_message>
<xml_diff>
--- a/uploads/shopping_slots_export.xlsx
+++ b/uploads/shopping_slots_export.xlsx
@@ -17,8 +17,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="yyyy-mm-dd"/>
-    <numFmt numFmtId="165" formatCode="YYYY-MM-DD"/>
+    <numFmt numFmtId="164" formatCode="yyyy-mm-dd h:mm:ss"/>
+    <numFmt numFmtId="165" formatCode="YYYY-MM-DD HH:MM:SS"/>
   </numFmts>
   <fonts count="2">
     <font>
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M11"/>
+  <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -445,60 +445,50 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>대행사</t>
+          <t>스토어 타입</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>스토어 타입</t>
+          <t>상품 ID</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>상품 ID</t>
+          <t>상품명</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>상품명</t>
+          <t>키워드</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>키워드</t>
+          <t>가격</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>가격</t>
+          <t>할인가</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>할인가</t>
+          <t>시작일</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>시작일</t>
+          <t>종료일</t>
         </is>
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
-          <t>종료일</t>
+          <t>입찰방식</t>
         </is>
       </c>
       <c r="K1" s="1" t="inlineStr">
-        <is>
-          <t>입찰방식</t>
-        </is>
-      </c>
-      <c r="L1" s="1" t="inlineStr">
-        <is>
-          <t>상태</t>
-        </is>
-      </c>
-      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>슬롯 단가</t>
         </is>
@@ -507,331 +497,95 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>이이이 Shopping 슬롯 20250506-1</t>
+          <t>샘플 슬롯 1</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>이이이</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr"/>
-      <c r="D2" t="inlineStr"/>
-      <c r="E2" t="inlineStr"/>
-      <c r="F2" t="inlineStr"/>
-      <c r="G2" t="inlineStr"/>
-      <c r="H2" t="inlineStr"/>
+          <t>스마트스토어</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>P12345</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>샘플 상품 1</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>키워드1,키워드2</t>
+        </is>
+      </c>
+      <c r="F2" t="n">
+        <v>10000</v>
+      </c>
+      <c r="G2" t="n">
+        <v>8000</v>
+      </c>
+      <c r="H2" s="2" t="n">
+        <v>45778</v>
+      </c>
       <c r="I2" s="2" t="n">
-        <v>45784</v>
-      </c>
-      <c r="J2" s="2" t="n">
-        <v>45786</v>
-      </c>
-      <c r="K2" t="inlineStr"/>
-      <c r="L2" t="inlineStr">
-        <is>
-          <t>live</t>
-        </is>
-      </c>
-      <c r="M2" t="n">
-        <v>30</v>
+        <v>45808</v>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>CPC</t>
+        </is>
+      </c>
+      <c r="K2" t="n">
+        <v>500</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>이이이 Shopping 슬롯 20250506-2</t>
+          <t>샘플 슬롯 2</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>이이이</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr"/>
-      <c r="D3" t="inlineStr"/>
-      <c r="E3" t="inlineStr"/>
-      <c r="F3" t="inlineStr"/>
-      <c r="G3" t="inlineStr"/>
-      <c r="H3" t="inlineStr"/>
+          <t>브랜드몰</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>P67890</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>샘플 상품 2</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>키워드3,키워드4</t>
+        </is>
+      </c>
+      <c r="F3" t="n">
+        <v>20000</v>
+      </c>
+      <c r="G3" t="n">
+        <v>18000</v>
+      </c>
+      <c r="H3" s="2" t="n">
+        <v>45792</v>
+      </c>
       <c r="I3" s="2" t="n">
-        <v>45784</v>
-      </c>
-      <c r="J3" s="2" t="n">
-        <v>45786</v>
-      </c>
-      <c r="K3" t="inlineStr"/>
-      <c r="L3" t="inlineStr">
-        <is>
-          <t>live</t>
-        </is>
-      </c>
-      <c r="M3" t="n">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>이이이 Shopping 슬롯 20250506-3</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>이이이</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr"/>
-      <c r="D4" t="inlineStr"/>
-      <c r="E4" t="inlineStr"/>
-      <c r="F4" t="inlineStr"/>
-      <c r="G4" t="inlineStr"/>
-      <c r="H4" t="inlineStr"/>
-      <c r="I4" s="2" t="n">
-        <v>45784</v>
-      </c>
-      <c r="J4" s="2" t="n">
-        <v>45786</v>
-      </c>
-      <c r="K4" t="inlineStr"/>
-      <c r="L4" t="inlineStr">
-        <is>
-          <t>live</t>
-        </is>
-      </c>
-      <c r="M4" t="n">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>이이이 Shopping 슬롯 20250506-4</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>이이이</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr"/>
-      <c r="D5" t="inlineStr"/>
-      <c r="E5" t="inlineStr"/>
-      <c r="F5" t="inlineStr"/>
-      <c r="G5" t="inlineStr"/>
-      <c r="H5" t="inlineStr"/>
-      <c r="I5" s="2" t="n">
-        <v>45784</v>
-      </c>
-      <c r="J5" s="2" t="n">
-        <v>45786</v>
-      </c>
-      <c r="K5" t="inlineStr"/>
-      <c r="L5" t="inlineStr">
-        <is>
-          <t>live</t>
-        </is>
-      </c>
-      <c r="M5" t="n">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>이이이 Shopping 슬롯 20250506-5</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>이이이</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr"/>
-      <c r="D6" t="inlineStr"/>
-      <c r="E6" t="inlineStr"/>
-      <c r="F6" t="inlineStr"/>
-      <c r="G6" t="inlineStr"/>
-      <c r="H6" t="inlineStr"/>
-      <c r="I6" s="2" t="n">
-        <v>45784</v>
-      </c>
-      <c r="J6" s="2" t="n">
-        <v>45786</v>
-      </c>
-      <c r="K6" t="inlineStr"/>
-      <c r="L6" t="inlineStr">
-        <is>
-          <t>live</t>
-        </is>
-      </c>
-      <c r="M6" t="n">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>이이이 Shopping 슬롯 20250506-6</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>이이이</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr"/>
-      <c r="D7" t="inlineStr"/>
-      <c r="E7" t="inlineStr"/>
-      <c r="F7" t="inlineStr"/>
-      <c r="G7" t="inlineStr"/>
-      <c r="H7" t="inlineStr"/>
-      <c r="I7" s="2" t="n">
-        <v>45784</v>
-      </c>
-      <c r="J7" s="2" t="n">
-        <v>45786</v>
-      </c>
-      <c r="K7" t="inlineStr"/>
-      <c r="L7" t="inlineStr">
-        <is>
-          <t>live</t>
-        </is>
-      </c>
-      <c r="M7" t="n">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>이이이 Shopping 슬롯 20250506-7</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>이이이</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr"/>
-      <c r="D8" t="inlineStr"/>
-      <c r="E8" t="inlineStr"/>
-      <c r="F8" t="inlineStr"/>
-      <c r="G8" t="inlineStr"/>
-      <c r="H8" t="inlineStr"/>
-      <c r="I8" s="2" t="n">
-        <v>45784</v>
-      </c>
-      <c r="J8" s="2" t="n">
-        <v>45786</v>
-      </c>
-      <c r="K8" t="inlineStr"/>
-      <c r="L8" t="inlineStr">
-        <is>
-          <t>live</t>
-        </is>
-      </c>
-      <c r="M8" t="n">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>이이이 Shopping 슬롯 20250506-8</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>이이이</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr"/>
-      <c r="D9" t="inlineStr"/>
-      <c r="E9" t="inlineStr"/>
-      <c r="F9" t="inlineStr"/>
-      <c r="G9" t="inlineStr"/>
-      <c r="H9" t="inlineStr"/>
-      <c r="I9" s="2" t="n">
-        <v>45784</v>
-      </c>
-      <c r="J9" s="2" t="n">
-        <v>45786</v>
-      </c>
-      <c r="K9" t="inlineStr"/>
-      <c r="L9" t="inlineStr">
-        <is>
-          <t>live</t>
-        </is>
-      </c>
-      <c r="M9" t="n">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>이이이 Shopping 슬롯 20250506-9</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>이이이</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr"/>
-      <c r="D10" t="inlineStr"/>
-      <c r="E10" t="inlineStr"/>
-      <c r="F10" t="inlineStr"/>
-      <c r="G10" t="inlineStr"/>
-      <c r="H10" t="inlineStr"/>
-      <c r="I10" s="2" t="n">
-        <v>45784</v>
-      </c>
-      <c r="J10" s="2" t="n">
-        <v>45786</v>
-      </c>
-      <c r="K10" t="inlineStr"/>
-      <c r="L10" t="inlineStr">
-        <is>
-          <t>live</t>
-        </is>
-      </c>
-      <c r="M10" t="n">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>이이이 Shopping 슬롯 20250506-10</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>이이이</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr"/>
-      <c r="D11" t="inlineStr"/>
-      <c r="E11" t="inlineStr"/>
-      <c r="F11" t="inlineStr"/>
-      <c r="G11" t="inlineStr"/>
-      <c r="H11" t="inlineStr"/>
-      <c r="I11" s="2" t="n">
-        <v>45784</v>
-      </c>
-      <c r="J11" s="2" t="n">
-        <v>45786</v>
-      </c>
-      <c r="K11" t="inlineStr"/>
-      <c r="L11" t="inlineStr">
-        <is>
-          <t>live</t>
-        </is>
-      </c>
-      <c r="M11" t="n">
-        <v>30</v>
+        <v>45823</v>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>CPM</t>
+        </is>
+      </c>
+      <c r="K3" t="n">
+        <v>800</v>
       </c>
     </row>
   </sheetData>

</xml_diff>